<commit_message>
modify the risk doc
</commit_message>
<xml_diff>
--- a/Risk Management Report.xlsx
+++ b/Risk Management Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\HU\CISC\594\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1B68ED-F41B-47A4-B2A8-5981C279BFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED01AF75-2964-4B16-A436-26787913041B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="3660" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
+    <workbookView xWindow="21510" yWindow="4140" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Risk number</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Have a function to give random name as default</t>
+  </si>
+  <si>
+    <t>Week2.4</t>
+  </si>
+  <si>
+    <t>Duplicated cards</t>
+  </si>
+  <si>
+    <t>use a loop and iterate only once to prevent it from happening</t>
   </si>
 </sst>
 </file>
@@ -512,7 +521,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,12 +674,24 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>

</xml_diff>

<commit_message>
player class adjusted, game can be initialized
</commit_message>
<xml_diff>
--- a/Risk Management Report.xlsx
+++ b/Risk Management Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\HU\CISC\594\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED01AF75-2964-4B16-A436-26787913041B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E764A41-C006-4CF0-8228-C91D43BA79D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21510" yWindow="4140" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
+    <workbookView xWindow="5445" yWindow="3960" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Risk number</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>use a loop and iterate only once to prevent it from happening</t>
+  </si>
+  <si>
+    <t>Week2.5</t>
+  </si>
+  <si>
+    <t>Other players knows which card is suppressed</t>
+  </si>
+  <si>
+    <t>Need to create a new random code for each new game for each card, different from the card ID</t>
   </si>
 </sst>
 </file>
@@ -521,7 +530,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,12 +703,24 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add week 4 docs
</commit_message>
<xml_diff>
--- a/Risk Management Report.xlsx
+++ b/Risk Management Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\HU\CISC\594\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADFFF499-51FE-49BB-A4A8-9B79575C863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7930D748-4FBF-4BB0-AA38-8752128C912E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22020" yWindow="4485" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
+    <workbookView xWindow="28770" yWindow="3300" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Risk number</t>
   </si>
@@ -143,7 +143,34 @@
     <t>need to check availability first before allowing player to suppress</t>
   </si>
   <si>
-    <t>no</t>
+    <t>Week2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player issues card which is not available </t>
+  </si>
+  <si>
+    <t>check availability first</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Week3.2</t>
+  </si>
+  <si>
+    <t>Player issues card which is on board</t>
+  </si>
+  <si>
+    <t>if a card is onboard, it is not available</t>
+  </si>
+  <si>
+    <t>Week3.3</t>
+  </si>
+  <si>
+    <t>Player input the card code which doesn't belong to him/her</t>
+  </si>
+  <si>
+    <t>Use a while loop, if not legal, let the player do it again.</t>
   </si>
 </sst>
 </file>
@@ -214,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -232,18 +259,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -561,20 +576,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B6186A-11C0-49A1-AA28-B0A2F37D4186}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="20" style="6" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" style="6" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="6"/>
-    <col min="6" max="6" width="54.5703125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="54.5703125" style="7" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -786,26 +801,95 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>12</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="9">
-        <v>4</v>
-      </c>
-      <c r="D10" s="9">
-        <v>3</v>
-      </c>
-      <c r="E10" s="9">
-        <v>12</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>35</v>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4</v>
+      </c>
+      <c r="E11" s="6">
+        <v>8</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6">
+        <v>8</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6">
+        <v>16</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added on last piece, the game is going! v2.0.0
</commit_message>
<xml_diff>
--- a/Risk Management Report.xlsx
+++ b/Risk Management Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\HU\CISC\594\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7930D748-4FBF-4BB0-AA38-8752128C912E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8D1CDB0-20F7-4DD1-B777-75567D60E73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28770" yWindow="3300" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
+    <workbookView xWindow="2145" yWindow="3030" windowWidth="21600" windowHeight="15435" xr2:uid="{DEF087AA-608B-4179-B920-921219C0CC4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Risk number</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Use a while loop, if not legal, let the player do it again.</t>
+  </si>
+  <si>
+    <t>Week4.1</t>
+  </si>
+  <si>
+    <t>Game doesn't end when player has no card</t>
+  </si>
+  <si>
+    <t>only limit to 13 rounds</t>
   </si>
 </sst>
 </file>
@@ -576,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B6186A-11C0-49A1-AA28-B0A2F37D4186}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,6 +901,29 @@
         <v>38</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>